<commit_message>
decoding of CAN done,detection of EOF done,automatic trigering done,more testing to be done
</commit_message>
<xml_diff>
--- a/ukrcavanje/UkrcavanjeSpisak2018-19_Pavkovic.xlsx
+++ b/ukrcavanje/UkrcavanjeSpisak2018-19_Pavkovic.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\samba03\nastavni_materijali\ukrcavanje\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="460" windowWidth="24380" windowHeight="15540"/>
+    <workbookView xWindow="1215" yWindow="465" windowWidth="24375" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Studenti-Mentori-Teme" sheetId="1" r:id="rId1"/>
@@ -18,9 +13,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Studenti-Mentori-Teme'!$A$2:$P$262</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="118">
   <si>
     <t>Student</t>
   </si>
@@ -374,13 +369,22 @@
   </si>
   <si>
     <t>Jedno rešenje programske podrške za trajno i bezbedno čuvanje podataka u automobilskoj industriji</t>
+  </si>
+  <si>
+    <t>verovatnoca</t>
+  </si>
+  <si>
+    <t>SAU</t>
+  </si>
+  <si>
+    <t>analiza 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,7 +618,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -649,7 +653,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -826,43 +830,43 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P272"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E102" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E219" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J104" sqref="J104"/>
+      <selection pane="bottomRight" activeCell="B233" sqref="B233"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.453125" style="1"/>
+    <col min="1" max="1" width="8.42578125" style="1"/>
     <col min="2" max="2" width="20" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.81640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" style="1" customWidth="1"/>
-    <col min="12" max="13" width="15.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="26" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="26" customFormat="1" ht="15.75">
       <c r="A1" s="24" t="s">
         <v>67</v>
       </c>
@@ -895,7 +899,7 @@
       <c r="O1" s="24"/>
       <c r="P1" s="24"/>
     </row>
-    <row r="2" spans="1:16" ht="93.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="93.6" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -945,7 +949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16">
       <c r="A3" s="19">
         <v>1</v>
       </c>
@@ -975,7 +979,7 @@
       <c r="O3" s="19"/>
       <c r="P3" s="19"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16">
       <c r="A4" s="19">
         <v>1</v>
       </c>
@@ -1001,7 +1005,7 @@
       <c r="O4" s="19"/>
       <c r="P4" s="19"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16">
       <c r="A5" s="19">
         <v>1</v>
       </c>
@@ -1027,7 +1031,7 @@
       <c r="O5" s="19"/>
       <c r="P5" s="19"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16">
       <c r="A6" s="19">
         <v>1</v>
       </c>
@@ -1053,7 +1057,7 @@
       <c r="O6" s="19"/>
       <c r="P6" s="19"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16">
       <c r="A7" s="19">
         <v>1</v>
       </c>
@@ -1079,7 +1083,7 @@
       <c r="O7" s="19"/>
       <c r="P7" s="19"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16">
       <c r="A8" s="19">
         <v>1</v>
       </c>
@@ -1101,7 +1105,7 @@
       <c r="O8" s="19"/>
       <c r="P8" s="19"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16">
       <c r="A9" s="19">
         <v>1</v>
       </c>
@@ -1123,7 +1127,7 @@
       <c r="O9" s="19"/>
       <c r="P9" s="19"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16">
       <c r="A10" s="19">
         <v>1</v>
       </c>
@@ -1145,7 +1149,7 @@
       <c r="O10" s="19"/>
       <c r="P10" s="19"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16">
       <c r="A11" s="19">
         <v>1</v>
       </c>
@@ -1167,7 +1171,7 @@
       <c r="O11" s="19"/>
       <c r="P11" s="19"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16">
       <c r="A12" s="19">
         <v>1</v>
       </c>
@@ -1189,7 +1193,7 @@
       <c r="O12" s="19"/>
       <c r="P12" s="19"/>
     </row>
-    <row r="13" spans="1:16" s="5" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" s="5" customFormat="1" ht="41.1" customHeight="1">
       <c r="A13" s="20">
         <v>2</v>
       </c>
@@ -1219,7 +1223,7 @@
       <c r="O13" s="20"/>
       <c r="P13" s="20"/>
     </row>
-    <row r="14" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" s="5" customFormat="1">
       <c r="A14" s="20">
         <v>2</v>
       </c>
@@ -1245,7 +1249,7 @@
       <c r="O14" s="20"/>
       <c r="P14" s="20"/>
     </row>
-    <row r="15" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" s="5" customFormat="1">
       <c r="A15" s="20">
         <v>2</v>
       </c>
@@ -1271,7 +1275,7 @@
       <c r="O15" s="20"/>
       <c r="P15" s="20"/>
     </row>
-    <row r="16" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" s="5" customFormat="1">
       <c r="A16" s="20">
         <v>2</v>
       </c>
@@ -1297,7 +1301,7 @@
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
     </row>
-    <row r="17" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" s="5" customFormat="1">
       <c r="A17" s="20">
         <v>2</v>
       </c>
@@ -1323,7 +1327,7 @@
       <c r="O17" s="20"/>
       <c r="P17" s="20"/>
     </row>
-    <row r="18" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" s="5" customFormat="1">
       <c r="A18" s="20">
         <v>2</v>
       </c>
@@ -1345,7 +1349,7 @@
       <c r="O18" s="20"/>
       <c r="P18" s="20"/>
     </row>
-    <row r="19" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" s="5" customFormat="1">
       <c r="A19" s="20">
         <v>2</v>
       </c>
@@ -1367,7 +1371,7 @@
       <c r="O19" s="20"/>
       <c r="P19" s="20"/>
     </row>
-    <row r="20" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" s="5" customFormat="1">
       <c r="A20" s="20">
         <v>2</v>
       </c>
@@ -1389,7 +1393,7 @@
       <c r="O20" s="20"/>
       <c r="P20" s="20"/>
     </row>
-    <row r="21" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" s="5" customFormat="1">
       <c r="A21" s="20">
         <v>2</v>
       </c>
@@ -1411,7 +1415,7 @@
       <c r="O21" s="20"/>
       <c r="P21" s="20"/>
     </row>
-    <row r="22" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" s="5" customFormat="1">
       <c r="A22" s="20">
         <v>2</v>
       </c>
@@ -1433,7 +1437,7 @@
       <c r="O22" s="20"/>
       <c r="P22" s="20"/>
     </row>
-    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="15" customHeight="1">
       <c r="A23" s="19">
         <v>3</v>
       </c>
@@ -1463,7 +1467,7 @@
       <c r="O23" s="19"/>
       <c r="P23" s="19"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16">
       <c r="A24" s="19">
         <v>3</v>
       </c>
@@ -1489,7 +1493,7 @@
       <c r="O24" s="19"/>
       <c r="P24" s="19"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16">
       <c r="A25" s="19">
         <v>3</v>
       </c>
@@ -1515,7 +1519,7 @@
       <c r="O25" s="19"/>
       <c r="P25" s="19"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16">
       <c r="A26" s="19">
         <v>3</v>
       </c>
@@ -1541,7 +1545,7 @@
       <c r="O26" s="19"/>
       <c r="P26" s="19"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16">
       <c r="A27" s="19">
         <v>3</v>
       </c>
@@ -1567,7 +1571,7 @@
       <c r="O27" s="19"/>
       <c r="P27" s="19"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16">
       <c r="A28" s="19">
         <v>3</v>
       </c>
@@ -1589,7 +1593,7 @@
       <c r="O28" s="19"/>
       <c r="P28" s="19"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16">
       <c r="A29" s="19">
         <v>3</v>
       </c>
@@ -1611,7 +1615,7 @@
       <c r="O29" s="19"/>
       <c r="P29" s="19"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16">
       <c r="A30" s="19">
         <v>3</v>
       </c>
@@ -1633,7 +1637,7 @@
       <c r="O30" s="19"/>
       <c r="P30" s="19"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16">
       <c r="A31" s="19">
         <v>3</v>
       </c>
@@ -1655,7 +1659,7 @@
       <c r="O31" s="19"/>
       <c r="P31" s="19"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16">
       <c r="A32" s="19">
         <v>3</v>
       </c>
@@ -1677,7 +1681,7 @@
       <c r="O32" s="19"/>
       <c r="P32" s="19"/>
     </row>
-    <row r="33" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" ht="14.45" customHeight="1">
       <c r="A33" s="19">
         <v>5</v>
       </c>
@@ -1707,7 +1711,7 @@
       <c r="O33" s="19"/>
       <c r="P33" s="19"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16">
       <c r="A34" s="19">
         <v>5</v>
       </c>
@@ -1733,7 +1737,7 @@
       <c r="O34" s="19"/>
       <c r="P34" s="19"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16">
       <c r="A35" s="19">
         <v>5</v>
       </c>
@@ -1759,7 +1763,7 @@
       <c r="O35" s="19"/>
       <c r="P35" s="19"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16">
       <c r="A36" s="19">
         <v>5</v>
       </c>
@@ -1785,7 +1789,7 @@
       <c r="O36" s="19"/>
       <c r="P36" s="19"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16">
       <c r="A37" s="19">
         <v>5</v>
       </c>
@@ -1811,7 +1815,7 @@
       <c r="O37" s="19"/>
       <c r="P37" s="19"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16">
       <c r="A38" s="19">
         <v>5</v>
       </c>
@@ -1833,7 +1837,7 @@
       <c r="O38" s="19"/>
       <c r="P38" s="19"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16">
       <c r="A39" s="19">
         <v>5</v>
       </c>
@@ -1855,7 +1859,7 @@
       <c r="O39" s="19"/>
       <c r="P39" s="19"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16">
       <c r="A40" s="19">
         <v>5</v>
       </c>
@@ -1877,7 +1881,7 @@
       <c r="O40" s="19"/>
       <c r="P40" s="19"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16">
       <c r="A41" s="19">
         <v>5</v>
       </c>
@@ -1899,7 +1903,7 @@
       <c r="O41" s="19"/>
       <c r="P41" s="19"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16">
       <c r="A42" s="19">
         <v>5</v>
       </c>
@@ -1921,7 +1925,7 @@
       <c r="O42" s="19"/>
       <c r="P42" s="19"/>
     </row>
-    <row r="43" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" ht="14.45" customHeight="1">
       <c r="A43" s="19">
         <v>6</v>
       </c>
@@ -1951,7 +1955,7 @@
       <c r="O43" s="19"/>
       <c r="P43" s="19"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16">
       <c r="A44" s="19">
         <v>6</v>
       </c>
@@ -1977,7 +1981,7 @@
       <c r="O44" s="19"/>
       <c r="P44" s="19"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16">
       <c r="A45" s="19">
         <v>6</v>
       </c>
@@ -2003,7 +2007,7 @@
       <c r="O45" s="19"/>
       <c r="P45" s="19"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16">
       <c r="A46" s="19">
         <v>6</v>
       </c>
@@ -2029,7 +2033,7 @@
       <c r="O46" s="19"/>
       <c r="P46" s="19"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16">
       <c r="A47" s="19">
         <v>6</v>
       </c>
@@ -2055,7 +2059,7 @@
       <c r="O47" s="19"/>
       <c r="P47" s="19"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16">
       <c r="A48" s="19">
         <v>6</v>
       </c>
@@ -2077,7 +2081,7 @@
       <c r="O48" s="19"/>
       <c r="P48" s="19"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16">
       <c r="A49" s="19">
         <v>6</v>
       </c>
@@ -2099,7 +2103,7 @@
       <c r="O49" s="19"/>
       <c r="P49" s="19"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16">
       <c r="A50" s="19">
         <v>6</v>
       </c>
@@ -2121,7 +2125,7 @@
       <c r="O50" s="19"/>
       <c r="P50" s="19"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16">
       <c r="A51" s="19">
         <v>6</v>
       </c>
@@ -2143,7 +2147,7 @@
       <c r="O51" s="19"/>
       <c r="P51" s="19"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16">
       <c r="A52" s="19">
         <v>6</v>
       </c>
@@ -2165,7 +2169,7 @@
       <c r="O52" s="19"/>
       <c r="P52" s="19"/>
     </row>
-    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" ht="15" customHeight="1">
       <c r="A53" s="19">
         <v>7</v>
       </c>
@@ -2195,7 +2199,7 @@
       <c r="O53" s="19"/>
       <c r="P53" s="19"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16">
       <c r="A54" s="19">
         <v>7</v>
       </c>
@@ -2221,7 +2225,7 @@
       <c r="O54" s="19"/>
       <c r="P54" s="19"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16">
       <c r="A55" s="19">
         <v>7</v>
       </c>
@@ -2247,7 +2251,7 @@
       <c r="O55" s="19"/>
       <c r="P55" s="19"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16">
       <c r="A56" s="19">
         <v>7</v>
       </c>
@@ -2273,7 +2277,7 @@
       <c r="O56" s="19"/>
       <c r="P56" s="19"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16">
       <c r="A57" s="19">
         <v>7</v>
       </c>
@@ -2299,7 +2303,7 @@
       <c r="O57" s="19"/>
       <c r="P57" s="19"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16">
       <c r="A58" s="19">
         <v>7</v>
       </c>
@@ -2321,7 +2325,7 @@
       <c r="O58" s="19"/>
       <c r="P58" s="19"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16">
       <c r="A59" s="19">
         <v>7</v>
       </c>
@@ -2343,7 +2347,7 @@
       <c r="O59" s="19"/>
       <c r="P59" s="19"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16">
       <c r="A60" s="19">
         <v>7</v>
       </c>
@@ -2365,7 +2369,7 @@
       <c r="O60" s="19"/>
       <c r="P60" s="19"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16">
       <c r="A61" s="19">
         <v>7</v>
       </c>
@@ -2387,7 +2391,7 @@
       <c r="O61" s="19"/>
       <c r="P61" s="19"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16">
       <c r="A62" s="19">
         <v>7</v>
       </c>
@@ -2409,7 +2413,7 @@
       <c r="O62" s="19"/>
       <c r="P62" s="19"/>
     </row>
-    <row r="63" spans="1:16" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16" ht="51" customHeight="1">
       <c r="A63" s="19">
         <v>8</v>
       </c>
@@ -2439,7 +2443,7 @@
       <c r="O63" s="19"/>
       <c r="P63" s="19"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16">
       <c r="A64" s="19">
         <v>8</v>
       </c>
@@ -2465,7 +2469,7 @@
       <c r="O64" s="19"/>
       <c r="P64" s="19"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16">
       <c r="A65" s="19">
         <v>8</v>
       </c>
@@ -2491,7 +2495,7 @@
       <c r="O65" s="19"/>
       <c r="P65" s="19"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16">
       <c r="A66" s="19">
         <v>8</v>
       </c>
@@ -2517,7 +2521,7 @@
       <c r="O66" s="19"/>
       <c r="P66" s="19"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16">
       <c r="A67" s="19">
         <v>8</v>
       </c>
@@ -2543,7 +2547,7 @@
       <c r="O67" s="19"/>
       <c r="P67" s="19"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16">
       <c r="A68" s="19">
         <v>8</v>
       </c>
@@ -2565,7 +2569,7 @@
       <c r="O68" s="19"/>
       <c r="P68" s="19"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16">
       <c r="A69" s="19">
         <v>8</v>
       </c>
@@ -2587,7 +2591,7 @@
       <c r="O69" s="19"/>
       <c r="P69" s="19"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16">
       <c r="A70" s="19">
         <v>8</v>
       </c>
@@ -2609,7 +2613,7 @@
       <c r="O70" s="19"/>
       <c r="P70" s="19"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16">
       <c r="A71" s="19">
         <v>8</v>
       </c>
@@ -2631,7 +2635,7 @@
       <c r="O71" s="19"/>
       <c r="P71" s="19"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16">
       <c r="A72" s="19">
         <v>8</v>
       </c>
@@ -2653,7 +2657,7 @@
       <c r="O72" s="19"/>
       <c r="P72" s="19"/>
     </row>
-    <row r="73" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16" ht="54.95" customHeight="1">
       <c r="A73" s="19">
         <v>10</v>
       </c>
@@ -2685,7 +2689,7 @@
       <c r="O73" s="19"/>
       <c r="P73" s="19"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16">
       <c r="A74" s="19">
         <v>10</v>
       </c>
@@ -2711,7 +2715,7 @@
       <c r="O74" s="19"/>
       <c r="P74" s="19"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16">
       <c r="A75" s="19">
         <v>10</v>
       </c>
@@ -2737,7 +2741,7 @@
       <c r="O75" s="19"/>
       <c r="P75" s="19"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16">
       <c r="A76" s="19">
         <v>10</v>
       </c>
@@ -2763,7 +2767,7 @@
       <c r="O76" s="19"/>
       <c r="P76" s="19"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16">
       <c r="A77" s="19">
         <v>10</v>
       </c>
@@ -2789,7 +2793,7 @@
       <c r="O77" s="19"/>
       <c r="P77" s="19"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16">
       <c r="A78" s="19">
         <v>10</v>
       </c>
@@ -2811,7 +2815,7 @@
       <c r="O78" s="19"/>
       <c r="P78" s="19"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16">
       <c r="A79" s="19">
         <v>10</v>
       </c>
@@ -2833,7 +2837,7 @@
       <c r="O79" s="19"/>
       <c r="P79" s="19"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16">
       <c r="A80" s="19">
         <v>10</v>
       </c>
@@ -2855,7 +2859,7 @@
       <c r="O80" s="19"/>
       <c r="P80" s="19"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16">
       <c r="A81" s="19">
         <v>10</v>
       </c>
@@ -2877,7 +2881,7 @@
       <c r="O81" s="19"/>
       <c r="P81" s="19"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16">
       <c r="A82" s="19">
         <v>10</v>
       </c>
@@ -2899,7 +2903,7 @@
       <c r="O82" s="19"/>
       <c r="P82" s="19"/>
     </row>
-    <row r="83" spans="1:16" ht="116" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" ht="120">
       <c r="A83" s="17">
         <v>11</v>
       </c>
@@ -2937,7 +2941,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16">
       <c r="A84" s="17">
         <v>11</v>
       </c>
@@ -2959,7 +2963,7 @@
       <c r="O84" s="17"/>
       <c r="P84" s="17"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:16">
       <c r="A85" s="17">
         <v>11</v>
       </c>
@@ -2981,7 +2985,7 @@
       <c r="O85" s="17"/>
       <c r="P85" s="17"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16">
       <c r="A86" s="17">
         <v>11</v>
       </c>
@@ -3003,7 +3007,7 @@
       <c r="O86" s="17"/>
       <c r="P86" s="17"/>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16">
       <c r="A87" s="17">
         <v>11</v>
       </c>
@@ -3025,7 +3029,7 @@
       <c r="O87" s="17"/>
       <c r="P87" s="17"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16">
       <c r="A88" s="17">
         <v>11</v>
       </c>
@@ -3047,7 +3051,7 @@
       <c r="O88" s="17"/>
       <c r="P88" s="17"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:16">
       <c r="A89" s="17">
         <v>11</v>
       </c>
@@ -3069,7 +3073,7 @@
       <c r="O89" s="17"/>
       <c r="P89" s="17"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:16">
       <c r="A90" s="17">
         <v>11</v>
       </c>
@@ -3091,7 +3095,7 @@
       <c r="O90" s="17"/>
       <c r="P90" s="17"/>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:16">
       <c r="A91" s="17">
         <v>11</v>
       </c>
@@ -3113,7 +3117,7 @@
       <c r="O91" s="17"/>
       <c r="P91" s="17"/>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:16">
       <c r="A92" s="17">
         <v>11</v>
       </c>
@@ -3135,7 +3139,7 @@
       <c r="O92" s="17"/>
       <c r="P92" s="17"/>
     </row>
-    <row r="93" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:16" ht="57" customHeight="1">
       <c r="A93" s="17">
         <v>13</v>
       </c>
@@ -3167,7 +3171,7 @@
       <c r="O93" s="17"/>
       <c r="P93" s="17"/>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:16">
       <c r="A94" s="17">
         <v>13</v>
       </c>
@@ -3191,7 +3195,7 @@
       <c r="O94" s="17"/>
       <c r="P94" s="17"/>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:16">
       <c r="A95" s="17">
         <v>13</v>
       </c>
@@ -3215,7 +3219,7 @@
       <c r="O95" s="17"/>
       <c r="P95" s="17"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:16">
       <c r="A96" s="17">
         <v>13</v>
       </c>
@@ -3237,7 +3241,7 @@
       <c r="O96" s="17"/>
       <c r="P96" s="17"/>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:16">
       <c r="A97" s="17">
         <v>13</v>
       </c>
@@ -3261,7 +3265,7 @@
       <c r="O97" s="17"/>
       <c r="P97" s="17"/>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16">
       <c r="A98" s="17">
         <v>13</v>
       </c>
@@ -3283,7 +3287,7 @@
       <c r="O98" s="17"/>
       <c r="P98" s="17"/>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16">
       <c r="A99" s="17">
         <v>13</v>
       </c>
@@ -3305,7 +3309,7 @@
       <c r="O99" s="17"/>
       <c r="P99" s="17"/>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16">
       <c r="A100" s="17">
         <v>13</v>
       </c>
@@ -3327,7 +3331,7 @@
       <c r="O100" s="17"/>
       <c r="P100" s="17"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:16">
       <c r="A101" s="17">
         <v>13</v>
       </c>
@@ -3349,7 +3353,7 @@
       <c r="O101" s="17"/>
       <c r="P101" s="17"/>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:16">
       <c r="A102" s="17">
         <v>13</v>
       </c>
@@ -3371,7 +3375,7 @@
       <c r="O102" s="17"/>
       <c r="P102" s="17"/>
     </row>
-    <row r="103" spans="1:16" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:16" ht="57.95" customHeight="1">
       <c r="A103" s="17">
         <v>14</v>
       </c>
@@ -3400,7 +3404,7 @@
       <c r="O103" s="17"/>
       <c r="P103" s="17"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:16">
       <c r="A104" s="17">
         <v>14</v>
       </c>
@@ -3426,7 +3430,7 @@
       <c r="O104" s="17"/>
       <c r="P104" s="17"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:16">
       <c r="A105" s="17">
         <v>14</v>
       </c>
@@ -3452,7 +3456,7 @@
       <c r="O105" s="17"/>
       <c r="P105" s="17"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:16">
       <c r="A106" s="17">
         <v>14</v>
       </c>
@@ -3478,7 +3482,7 @@
       <c r="O106" s="17"/>
       <c r="P106" s="17"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:16">
       <c r="A107" s="17">
         <v>14</v>
       </c>
@@ -3504,7 +3508,7 @@
       <c r="O107" s="17"/>
       <c r="P107" s="17"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:16">
       <c r="A108" s="17">
         <v>14</v>
       </c>
@@ -3526,7 +3530,7 @@
       <c r="O108" s="17"/>
       <c r="P108" s="17"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:16">
       <c r="A109" s="17">
         <v>14</v>
       </c>
@@ -3548,7 +3552,7 @@
       <c r="O109" s="17"/>
       <c r="P109" s="17"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:16">
       <c r="A110" s="17">
         <v>14</v>
       </c>
@@ -3570,7 +3574,7 @@
       <c r="O110" s="17"/>
       <c r="P110" s="17"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:16">
       <c r="A111" s="17">
         <v>14</v>
       </c>
@@ -3592,7 +3596,7 @@
       <c r="O111" s="17"/>
       <c r="P111" s="17"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:16">
       <c r="A112" s="17">
         <v>14</v>
       </c>
@@ -3614,7 +3618,7 @@
       <c r="O112" s="17"/>
       <c r="P112" s="17"/>
     </row>
-    <row r="113" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:16" ht="72" customHeight="1">
       <c r="A113" s="17">
         <v>15</v>
       </c>
@@ -3648,7 +3652,7 @@
       <c r="O113" s="17"/>
       <c r="P113" s="17"/>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:16">
       <c r="A114" s="17">
         <v>15</v>
       </c>
@@ -3672,7 +3676,7 @@
       <c r="O114" s="17"/>
       <c r="P114" s="17"/>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:16">
       <c r="A115" s="17">
         <v>15</v>
       </c>
@@ -3696,7 +3700,7 @@
       <c r="O115" s="17"/>
       <c r="P115" s="17"/>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:16">
       <c r="A116" s="17">
         <v>15</v>
       </c>
@@ -3720,7 +3724,7 @@
       <c r="O116" s="17"/>
       <c r="P116" s="17"/>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:16">
       <c r="A117" s="17">
         <v>15</v>
       </c>
@@ -3744,7 +3748,7 @@
       <c r="O117" s="17"/>
       <c r="P117" s="17"/>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:16">
       <c r="A118" s="17">
         <v>15</v>
       </c>
@@ -3766,7 +3770,7 @@
       <c r="O118" s="17"/>
       <c r="P118" s="17"/>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:16">
       <c r="A119" s="17">
         <v>15</v>
       </c>
@@ -3788,7 +3792,7 @@
       <c r="O119" s="17"/>
       <c r="P119" s="17"/>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:16">
       <c r="A120" s="17">
         <v>15</v>
       </c>
@@ -3810,7 +3814,7 @@
       <c r="O120" s="17"/>
       <c r="P120" s="17"/>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:16">
       <c r="A121" s="17">
         <v>15</v>
       </c>
@@ -3832,7 +3836,7 @@
       <c r="O121" s="17"/>
       <c r="P121" s="17"/>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:16">
       <c r="A122" s="17">
         <v>15</v>
       </c>
@@ -3854,7 +3858,7 @@
       <c r="O122" s="17"/>
       <c r="P122" s="17"/>
     </row>
-    <row r="123" spans="1:16" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:16" ht="69" customHeight="1">
       <c r="A123" s="17">
         <v>16</v>
       </c>
@@ -3865,7 +3869,7 @@
       <c r="O123" s="17"/>
       <c r="P123" s="17"/>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:16">
       <c r="A124" s="17">
         <v>16</v>
       </c>
@@ -3877,7 +3881,7 @@
       <c r="O124" s="17"/>
       <c r="P124" s="17"/>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:16">
       <c r="A125" s="17">
         <v>16</v>
       </c>
@@ -3889,7 +3893,7 @@
       <c r="O125" s="17"/>
       <c r="P125" s="17"/>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:16">
       <c r="A126" s="17">
         <v>16</v>
       </c>
@@ -3901,7 +3905,7 @@
       <c r="O126" s="17"/>
       <c r="P126" s="17"/>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:16">
       <c r="A127" s="17">
         <v>16</v>
       </c>
@@ -3913,7 +3917,7 @@
       <c r="O127" s="17"/>
       <c r="P127" s="17"/>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:16">
       <c r="A128" s="17">
         <v>16</v>
       </c>
@@ -3925,7 +3929,7 @@
       <c r="O128" s="17"/>
       <c r="P128" s="17"/>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:16">
       <c r="A129" s="17">
         <v>16</v>
       </c>
@@ -3937,7 +3941,7 @@
       <c r="O129" s="17"/>
       <c r="P129" s="17"/>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:16">
       <c r="A130" s="17">
         <v>16</v>
       </c>
@@ -3949,7 +3953,7 @@
       <c r="O130" s="17"/>
       <c r="P130" s="17"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:16">
       <c r="A131" s="17">
         <v>16</v>
       </c>
@@ -3961,7 +3965,7 @@
       <c r="O131" s="17"/>
       <c r="P131" s="17"/>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:16">
       <c r="A132" s="17">
         <v>16</v>
       </c>
@@ -3973,7 +3977,7 @@
       <c r="O132" s="17"/>
       <c r="P132" s="17"/>
     </row>
-    <row r="133" spans="1:16" ht="87" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:16" ht="120">
       <c r="A133" s="17">
         <v>17</v>
       </c>
@@ -4007,7 +4011,7 @@
       <c r="O133" s="17"/>
       <c r="P133" s="17"/>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:16">
       <c r="A134" s="17">
         <v>17</v>
       </c>
@@ -4029,7 +4033,7 @@
       <c r="O134" s="17"/>
       <c r="P134" s="17"/>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:16">
       <c r="A135" s="17">
         <v>17</v>
       </c>
@@ -4051,7 +4055,7 @@
       <c r="O135" s="17"/>
       <c r="P135" s="17"/>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:16">
       <c r="A136" s="17">
         <v>17</v>
       </c>
@@ -4073,7 +4077,7 @@
       <c r="O136" s="17"/>
       <c r="P136" s="17"/>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:16">
       <c r="A137" s="17">
         <v>17</v>
       </c>
@@ -4095,7 +4099,7 @@
       <c r="O137" s="17"/>
       <c r="P137" s="17"/>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:16">
       <c r="A138" s="17">
         <v>17</v>
       </c>
@@ -4117,7 +4121,7 @@
       <c r="O138" s="17"/>
       <c r="P138" s="17"/>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:16">
       <c r="A139" s="17">
         <v>17</v>
       </c>
@@ -4139,7 +4143,7 @@
       <c r="O139" s="17"/>
       <c r="P139" s="17"/>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:16">
       <c r="A140" s="17">
         <v>17</v>
       </c>
@@ -4161,7 +4165,7 @@
       <c r="O140" s="17"/>
       <c r="P140" s="17"/>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:16">
       <c r="A141" s="17">
         <v>17</v>
       </c>
@@ -4183,7 +4187,7 @@
       <c r="O141" s="17"/>
       <c r="P141" s="17"/>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:16">
       <c r="A142" s="17">
         <v>17</v>
       </c>
@@ -4205,7 +4209,7 @@
       <c r="O142" s="17"/>
       <c r="P142" s="17"/>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:16">
       <c r="B143" s="1" t="s">
         <v>79</v>
       </c>
@@ -4216,52 +4220,52 @@
         <v>43469</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:16">
       <c r="A144" s="27">
         <v>18</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:12">
       <c r="A145" s="27">
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:12">
       <c r="A146" s="27">
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:12">
       <c r="A147" s="27">
         <v>18</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:12">
       <c r="A148" s="27">
         <v>18</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:12">
       <c r="A149" s="27">
         <v>18</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:12">
       <c r="A150" s="27">
         <v>18</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:12">
       <c r="A151" s="27">
         <v>18</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:12">
       <c r="A152" s="27">
         <v>18</v>
       </c>
     </row>
-    <row r="153" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:12" ht="75">
       <c r="B153" s="1" t="s">
         <v>81</v>
       </c>
@@ -4275,52 +4279,52 @@
         <v>101</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:12">
       <c r="A154" s="27">
         <v>19</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:12">
       <c r="A155" s="27">
         <v>19</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:12">
       <c r="A156" s="27">
         <v>19</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:12">
       <c r="A157" s="27">
         <v>19</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:12">
       <c r="A158" s="27">
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:12">
       <c r="A159" s="27">
         <v>19</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:12">
       <c r="A160" s="27">
         <v>19</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:12">
       <c r="A161" s="27">
         <v>19</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:12">
       <c r="A162" s="27">
         <v>19</v>
       </c>
     </row>
-    <row r="163" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:12" ht="105">
       <c r="B163" s="1" t="s">
         <v>83</v>
       </c>
@@ -4334,52 +4338,52 @@
         <v>102</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:12">
       <c r="A164" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:12">
       <c r="A165" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12">
       <c r="A166" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12">
       <c r="A167" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:12">
       <c r="A168" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:12">
       <c r="A169" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:12">
       <c r="A170" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:12">
       <c r="A171" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:12">
       <c r="A172" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="173" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:12" ht="75">
       <c r="A173" s="27"/>
       <c r="B173" s="1" t="s">
         <v>84</v>
@@ -4394,52 +4398,52 @@
         <v>103</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:12">
       <c r="A174" s="27">
         <v>21</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:12">
       <c r="A175" s="27">
         <v>21</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:12">
       <c r="A176" s="27">
         <v>21</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:12">
       <c r="A177" s="27">
         <v>21</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:12">
       <c r="A178" s="27">
         <v>21</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:12">
       <c r="A179" s="27">
         <v>21</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:12">
       <c r="A180" s="27">
         <v>21</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:12">
       <c r="A181" s="27">
         <v>21</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:12">
       <c r="A182" s="27">
         <v>21</v>
       </c>
     </row>
-    <row r="183" spans="1:12" ht="116" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:12" ht="120">
       <c r="B183" s="1" t="s">
         <v>86</v>
       </c>
@@ -4453,52 +4457,52 @@
         <v>104</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:12">
       <c r="A184" s="27">
         <v>22</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:12">
       <c r="A185" s="27">
         <v>22</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:12">
       <c r="A186" s="27">
         <v>22</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:12">
       <c r="A187" s="27">
         <v>22</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:12">
       <c r="A188" s="27">
         <v>22</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:12">
       <c r="A189" s="27">
         <v>22</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:12">
       <c r="A190" s="27">
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:12">
       <c r="A191" s="27">
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:12">
       <c r="A192" s="27">
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:12" ht="75">
       <c r="B193" s="1" t="s">
         <v>88</v>
       </c>
@@ -4512,52 +4516,52 @@
         <v>105</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12">
       <c r="A194" s="27">
         <v>23</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12">
       <c r="A195" s="27">
         <v>23</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12">
       <c r="A196" s="27">
         <v>23</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:12">
       <c r="A197" s="27">
         <v>23</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12">
       <c r="A198" s="27">
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12">
       <c r="A199" s="27">
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:12">
       <c r="A200" s="27">
         <v>23</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:12">
       <c r="A201" s="27">
         <v>23</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12">
       <c r="A202" s="27">
         <v>23</v>
       </c>
     </row>
-    <row r="203" spans="1:12" ht="87" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" ht="90">
       <c r="B203" s="1" t="s">
         <v>90</v>
       </c>
@@ -4571,52 +4575,52 @@
         <v>106</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:12">
       <c r="A204" s="27">
         <v>24</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12">
       <c r="A205" s="27">
         <v>24</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:12">
       <c r="A206" s="27">
         <v>24</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:12">
       <c r="A207" s="27">
         <v>24</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:12">
       <c r="A208" s="27">
         <v>24</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:12">
       <c r="A209" s="27">
         <v>24</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:12">
       <c r="A210" s="27">
         <v>24</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:12">
       <c r="A211" s="27">
         <v>24</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:12">
       <c r="A212" s="27">
         <v>24</v>
       </c>
     </row>
-    <row r="213" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:12" ht="60">
       <c r="B213" s="1" t="s">
         <v>91</v>
       </c>
@@ -4630,52 +4634,52 @@
         <v>107</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:12">
       <c r="A214" s="27">
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:12">
       <c r="A215" s="27">
         <v>25</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:12">
       <c r="A216" s="27">
         <v>25</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:12">
       <c r="A217" s="27">
         <v>25</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:12">
       <c r="A218" s="27">
         <v>25</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:12">
       <c r="A219" s="27">
         <v>25</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:12">
       <c r="A220" s="27">
         <v>25</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:12">
       <c r="A221" s="27">
         <v>25</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:12">
       <c r="A222" s="27">
         <v>25</v>
       </c>
     </row>
-    <row r="223" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:12" ht="135">
       <c r="B223" s="1" t="s">
         <v>93</v>
       </c>
@@ -4689,52 +4693,55 @@
         <v>108</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:12">
       <c r="A224" s="27">
         <v>26</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:12">
       <c r="A225" s="27">
         <v>26</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:12">
       <c r="A226" s="27">
         <v>26</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:12">
       <c r="A227" s="27">
         <v>26</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:12">
       <c r="A228" s="27">
         <v>26</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:12">
       <c r="A229" s="27">
         <v>26</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:12">
       <c r="A230" s="27">
         <v>26</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:12">
       <c r="A231" s="27">
         <v>26</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:12">
       <c r="A232" s="27">
         <v>26</v>
       </c>
     </row>
-    <row r="233" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:12" ht="105">
+      <c r="A233" s="27">
+        <v>27</v>
+      </c>
       <c r="B233" s="1" t="s">
         <v>95</v>
       </c>
@@ -4744,56 +4751,65 @@
       <c r="F233" s="28">
         <v>43469</v>
       </c>
+      <c r="H233" s="10" t="s">
+        <v>115</v>
+      </c>
       <c r="L233" s="16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:12">
       <c r="A234" s="27">
         <v>27</v>
       </c>
-    </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H234" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12">
       <c r="A235" s="27">
         <v>27</v>
       </c>
-    </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H235" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12">
       <c r="A236" s="27">
         <v>27</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:12">
       <c r="A237" s="27">
         <v>27</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:12">
       <c r="A238" s="27">
         <v>27</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:12">
       <c r="A239" s="27">
         <v>27</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:12">
       <c r="A240" s="27">
         <v>27</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:12">
       <c r="A241" s="27">
         <v>27</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:12">
       <c r="A242" s="27">
         <v>27</v>
       </c>
     </row>
-    <row r="243" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:12" ht="150">
       <c r="B243" s="1" t="s">
         <v>97</v>
       </c>
@@ -4807,52 +4823,52 @@
         <v>110</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:12">
       <c r="A244" s="27">
         <v>28</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:12">
       <c r="A245" s="27">
         <v>28</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:12">
       <c r="A246" s="27">
         <v>28</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:12">
       <c r="A247" s="27">
         <v>28</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:12">
       <c r="A248" s="27">
         <v>28</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:12">
       <c r="A249" s="27">
         <v>28</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:12">
       <c r="A250" s="27">
         <v>28</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:12">
       <c r="A251" s="27">
         <v>28</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:12">
       <c r="A252" s="27">
         <v>28</v>
       </c>
     </row>
-    <row r="253" spans="1:12" ht="145" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:12" ht="165">
       <c r="B253" s="1" t="s">
         <v>99</v>
       </c>
@@ -4866,52 +4882,52 @@
         <v>111</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:12">
       <c r="A254" s="27">
         <v>29</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:12">
       <c r="A255" s="27">
         <v>29</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:12">
       <c r="A256" s="27">
         <v>29</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:12">
       <c r="A257" s="27">
         <v>29</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:12">
       <c r="A258" s="27">
         <v>29</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:12">
       <c r="A259" s="27">
         <v>29</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:12">
       <c r="A260" s="27">
         <v>29</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:12">
       <c r="A261" s="27">
         <v>29</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:12">
       <c r="A262" s="27">
         <v>29</v>
       </c>
     </row>
-    <row r="263" spans="1:12" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:12" ht="135">
       <c r="B263" s="1" t="s">
         <v>112</v>
       </c>
@@ -4929,47 +4945,47 @@
         <v>114</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:12">
       <c r="A264" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:12">
       <c r="A265" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:12">
       <c r="A266" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:12">
       <c r="A267" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:12">
       <c r="A268" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:12">
       <c r="A269" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:12">
       <c r="A270" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:12">
       <c r="A271" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:12">
       <c r="A272" s="1">
         <v>30</v>
       </c>
@@ -4982,21 +4998,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:D6"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.453125" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:4" ht="21">
       <c r="B1" s="13" t="s">
         <v>49</v>
       </c>
@@ -5007,7 +5023,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="30">
       <c r="B2" s="12" t="s">
         <v>48</v>
       </c>
@@ -5018,7 +5034,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:4">
       <c r="B3" t="s">
         <v>56</v>
       </c>
@@ -5029,7 +5045,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4">
       <c r="B4" t="s">
         <v>57</v>
       </c>
@@ -5040,7 +5056,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
         <v>58</v>
       </c>
@@ -5051,7 +5067,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4">
       <c r="B6" t="s">
         <v>64</v>
       </c>

</xml_diff>